<commit_message>
atualizando as planilhas de instruções e componestes do processador
</commit_message>
<xml_diff>
--- a/Controle de componentes do Processador.xlsx
+++ b/Controle de componentes do Processador.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Wanderson\UEFS\SD\git\ANTARES-R2_PBLSD\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="360" yWindow="75" windowWidth="15315" windowHeight="6210"/>
   </bookViews>
@@ -154,14 +159,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="14">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="5">
     <dxf>
       <fill>
         <patternFill>
@@ -191,56 +189,6 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill>
           <bgColor rgb="FF00B050"/>
@@ -252,6 +200,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -300,7 +251,7 @@
     </a:clrScheme>
     <a:fontScheme name="Escritório">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -335,7 +286,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -547,13 +498,13 @@
   <dimension ref="G2:J16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14:J14"/>
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="8" max="8" width="16.85546875" customWidth="1"/>
-    <col min="10" max="10" width="18.28515625" customWidth="1"/>
+    <col min="8" max="8" width="16.875" customWidth="1"/>
+    <col min="10" max="10" width="18.25" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="7:10" x14ac:dyDescent="0.25">
@@ -590,7 +541,7 @@
       </c>
       <c r="H5" s="2"/>
       <c r="I5" s="2" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="J5" s="2"/>
     </row>
@@ -600,7 +551,7 @@
       </c>
       <c r="H6" s="2"/>
       <c r="I6" s="2" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="J6" s="2"/>
     </row>
@@ -610,7 +561,7 @@
       </c>
       <c r="H7" s="2"/>
       <c r="I7" s="2" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="J7" s="2"/>
     </row>
@@ -620,7 +571,7 @@
       </c>
       <c r="H8" s="2"/>
       <c r="I8" s="2" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="J8" s="2"/>
     </row>
@@ -630,7 +581,7 @@
       </c>
       <c r="H9" s="2"/>
       <c r="I9" s="2" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="J9" s="2"/>
     </row>
@@ -640,7 +591,7 @@
       </c>
       <c r="H10" s="2"/>
       <c r="I10" s="2" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="J10" s="2"/>
     </row>
@@ -650,7 +601,7 @@
       </c>
       <c r="H11" s="2"/>
       <c r="I11" s="2" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="J11" s="2"/>
     </row>
@@ -660,7 +611,7 @@
       </c>
       <c r="H12" s="2"/>
       <c r="I12" s="2" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="J12" s="2"/>
     </row>
@@ -680,7 +631,7 @@
       </c>
       <c r="H14" s="2"/>
       <c r="I14" s="2" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="J14" s="2"/>
     </row>
@@ -700,27 +651,12 @@
       </c>
       <c r="H16" s="2"/>
       <c r="I16" s="2" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="J16" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="I12:J12"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="I13:J13"/>
-    <mergeCell ref="I14:J14"/>
-    <mergeCell ref="I15:J15"/>
-    <mergeCell ref="I16:J16"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="I4:J4"/>
-    <mergeCell ref="G5:H5"/>
     <mergeCell ref="G9:H9"/>
     <mergeCell ref="G10:H10"/>
     <mergeCell ref="G11:H11"/>
@@ -734,27 +670,42 @@
     <mergeCell ref="G6:H6"/>
     <mergeCell ref="G7:H7"/>
     <mergeCell ref="G8:H8"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="I13:J13"/>
+    <mergeCell ref="I14:J14"/>
+    <mergeCell ref="I15:J15"/>
+    <mergeCell ref="I16:J16"/>
   </mergeCells>
   <conditionalFormatting sqref="I4:J11">
-    <cfRule type="containsText" dxfId="13" priority="8" operator="containsText" text="Feito">
+    <cfRule type="containsText" dxfId="4" priority="8" operator="containsText" text="Feito">
       <formula>NOT(ISERROR(SEARCH("Feito",I4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="9" operator="containsText" text="A fazer">
+    <cfRule type="containsText" dxfId="3" priority="9" operator="containsText" text="A fazer">
       <formula>NOT(ISERROR(SEARCH("A fazer",I4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I13:J16">
-    <cfRule type="containsText" dxfId="9" priority="3" operator="containsText" text="A Fazer">
+    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="A Fazer">
       <formula>NOT(ISERROR(SEARCH("A Fazer",I13)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I12:J12">
-    <cfRule type="containsText" dxfId="3" priority="2" operator="containsText" text="A Fazer">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="A Fazer">
       <formula>NOT(ISERROR(SEARCH("A Fazer",I12)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I12:J16">
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="Feito">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="Feito">
       <formula>NOT(ISERROR(SEARCH("Feito",I12)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>